<commit_message>
[Form] - Single child scroll view
</commit_message>
<xml_diff>
--- a/Tutorial #/Form.xlsx
+++ b/Tutorial #/Form.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\Flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{601767CE-E3CF-4B04-B2F7-A8AE03FB0F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB78E9A6-2E42-4FE3-A3B0-E2E548BD701A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form" sheetId="1" r:id="rId1"/>
+    <sheet name="Single child scroll view proper" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <r>
       <rPr>
@@ -166,13 +167,53 @@
   <si>
     <t xml:space="preserve">text inputs , redio buttons , check box </t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Single child scroll view properly</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">මෙතන පේනවා අපේ design එක </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>cut වෙලා error එකක් එනවා</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Screen එක අනුව </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">design display වෙන විදි වෙනස් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ඒ හින්දා අපිට මේක </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">scroll කරන්න පුළුවන් විදියේ </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">desing එකක් ඕනේ වෙනවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ඒකට තමයි </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Single child scroll view </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">method use කරන්නේ </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -256,6 +297,14 @@
       <b/>
       <sz val="20"/>
       <color theme="9"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FF002060"/>
       <name val="游ゴシック"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -281,7 +330,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -289,6 +338,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -304,6 +354,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>111965</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>142936</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>449581</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>312419</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE34D110-4BD1-4266-88D5-13AE8B30F52C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="111965" y="4547296"/>
+          <a:ext cx="7713776" cy="5107243"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>373380</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>322023</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1893183-2285-42B4-8533-D99D868A3579}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="594360" y="10126980"/>
+          <a:ext cx="9786063" cy="5836920"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -571,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M9" sqref="M9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
@@ -610,4 +753,79 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EEFCA9-EE7F-4190-8508-BC0C5BFF0AEF}">
+  <dimension ref="A1:N15"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="21" customHeight="1" x14ac:dyDescent="0.8"/>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="M3" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="N4" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="M6" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="N7" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="M9" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="N10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="N11" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="M13" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="N14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.8">
+      <c r="N15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[Form] - Text Form Field ( validator:  |  onSaved : )
</commit_message>
<xml_diff>
--- a/Tutorial #/Form.xlsx
+++ b/Tutorial #/Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\Flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB78E9A6-2E42-4FE3-A3B0-E2E548BD701A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9C37DC-5B97-4ABC-B6FD-8811A7314758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
   <si>
     <r>
       <rPr>
@@ -208,12 +208,92 @@
   <si>
     <t xml:space="preserve">method use කරන්නේ </t>
   </si>
+  <si>
+    <t>key:</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Form එකේ විස්තර දැනගන්න use කරනවා </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>TextFormField()</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>validator :</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">මේක anonyms function එකක් විදියට තියෙන්නේ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">text field එකේ තියන value එක automatically මේ functions එකේ variable එකකට ගන්නව </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">මේකේ අනිවාර්යෙන්ම value එකක් return කරන්න ඕනේ </t>
+  </si>
+  <si>
+    <t>Error display</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>return null;</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">මේකෙන් අදහස් වෙන්නේ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මේ Field එකේ error එකක් නැ කියන එක </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>return "String text";</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">error එකක් තියනව </t>
+  </si>
+  <si>
+    <t xml:space="preserve">return වෙන string එක තමයි </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">error message එක වෙන්නේ </t>
+  </si>
+  <si>
+    <t>onSaved :</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">text form field එක හරියට validate වෙලා තියනවනම් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ඒ valid text එක system එකට ගන්නවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">form එකේ fields මොක්කොම vailed නම් විතරක් එකට වෙලාවේ ඒ ඔක්කොම values ටික අරගන්නවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මේක optional method එකක් </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මේක අනිවාර්යෙන් ලියන්න ඕනේ නැ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">මේක run වෙන්නේ form එකේ state එක save කරන වෙලාවේදී </t>
+  </si>
+  <si>
+    <t>save කරනවා කියන්නේ form එක btn එකකින් submit කරන වෙලාව</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +389,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FF7030A0"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="30"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="游ゴシック"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -330,7 +435,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -339,6 +444,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -357,6 +467,451 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>114301</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>102949</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>320041</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>35615</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DD5680A-95DE-D34C-D8D9-DD381DFD92E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2125981" y="4240609"/>
+          <a:ext cx="4899660" cy="3224506"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>198120</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>251460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>160997</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>5330</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{922B6FC9-E0A6-7426-7623-026ADA943F0A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="868680" y="8702040"/>
+          <a:ext cx="4656797" cy="2634230"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>251460</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>403628</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>534756</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>401627</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2327FE5-6985-F98F-6EF0-A872833AC9EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5615940" y="8854208"/>
+          <a:ext cx="3445596" cy="2055399"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>510540</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>376356</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>311048</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>381000</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DDB0CE54-AD33-358E-8786-905E335DABCC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9227820" y="8826936"/>
+          <a:ext cx="3823868" cy="2062044"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>652726</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>203622</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5545CB81-5F3E-F06B-5072-ECC021339ACA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId5"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="502920" y="12298680"/>
+          <a:ext cx="5514286" cy="1704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>56600</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>16963</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A31984D-1D07-AC7C-C109-2DA30C8ACAFF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6195060" y="11948160"/>
+          <a:ext cx="4400000" cy="1457143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>157573</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>79827</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1DB8697B-D04B-87D1-76AB-71089CBB2C35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId7"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9235440" y="12824460"/>
+          <a:ext cx="4333333" cy="1466667"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>251460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>237462</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>190148</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5322D019-37F3-9BD5-8809-D0EB6A6A6C90}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1638300" y="16718280"/>
+          <a:ext cx="5304762" cy="2819048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>297180</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>274320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323176</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>411118</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8D45BC3E-3B01-9F12-6F0F-5A18F20225BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="967740" y="20444460"/>
+          <a:ext cx="5390476" cy="2895238"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>182880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>203322</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>292996</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="11" name="Picture 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE164DF6-B6C2-B826-5A3F-9AA39AAEABDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="792480" y="26601420"/>
+          <a:ext cx="4104762" cy="2990476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -712,46 +1267,179 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:M68"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
   <cols>
-    <col min="1" max="16384" width="8.796875" style="1"/>
+    <col min="1" max="10" width="8.796875" style="1"/>
+    <col min="11" max="11" width="6.296875" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="51" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:4" ht="51" x14ac:dyDescent="0.8">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.8">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.8">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.8">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.8">
       <c r="B4" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.8">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.8">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.8">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.8">
       <c r="C7" s="4" t="s">
         <v>4</v>
       </c>
     </row>
+    <row r="9" spans="1:4" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B9" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B19" s="6" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="2:3" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B36" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.8">
+      <c r="C37" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.8">
+      <c r="C38" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="48" spans="2:3" x14ac:dyDescent="0.8">
+      <c r="C48" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="A49" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="A50" s="7"/>
+      <c r="K50" s="8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="A51" s="7"/>
+      <c r="L51" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="A52" s="7"/>
+      <c r="L52" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" ht="22.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A53" s="7"/>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="A54" s="7"/>
+      <c r="K54" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="A55" s="7"/>
+      <c r="L55" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="A56" s="7"/>
+      <c r="L56" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="L57" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="M58" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B59" s="6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="B60" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="C61" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="B62" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.8">
+      <c r="I64" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.8">
+      <c r="I65" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.8">
+      <c r="I67" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.8">
+      <c r="I68" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A49:A56"/>
+  </mergeCells>
   <phoneticPr fontId="3"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -759,7 +1447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EEFCA9-EE7F-4190-8508-BC0C5BFF0AEF}">
   <dimension ref="A1:N15"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
   <cols>

</xml_diff>

<commit_message>
[Form] - Check form validation
</commit_message>
<xml_diff>
--- a/Tutorial #/Form.xlsx
+++ b/Tutorial #/Form.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\Flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D9C37DC-5B97-4ABC-B6FD-8811A7314758}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16F8CE0-B2AD-42EF-B4E2-B92FE3FCE0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
   <si>
     <r>
       <rPr>
@@ -287,6 +287,18 @@
   </si>
   <si>
     <t>save කරනවා කියන්නේ form එක btn එකකින් submit කරන වෙලාව</t>
+  </si>
+  <si>
+    <t>BTN</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Form එක validate ද නැතිද කියලා check කරමු </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Form එක validate නම් values ටික අරගමු </t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -445,10 +457,10 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -900,6 +912,534 @@
         <a:xfrm>
           <a:off x="792480" y="26601420"/>
           <a:ext cx="4104762" cy="2990476"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>236220</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>358281</xdr:colOff>
+      <xdr:row>83</xdr:row>
+      <xdr:rowOff>393593</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{83713FAD-A069-7404-7E84-AD60F8AEB333}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="906780" y="30754320"/>
+          <a:ext cx="5486541" cy="4897013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>327660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>41303</xdr:colOff>
+      <xdr:row>82</xdr:row>
+      <xdr:rowOff>231908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="13" name="Picture 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2EC360C1-E9E3-4515-2E43-95B5AA87F3E3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7063740" y="31059120"/>
+          <a:ext cx="4857143" cy="4019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>274320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>208924</xdr:colOff>
+      <xdr:row>94</xdr:row>
+      <xdr:rowOff>216663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="14" name="Picture 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADC17DB9-53C6-DB5A-65E0-D383071257AC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1234440" y="35943540"/>
+          <a:ext cx="5009524" cy="4057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>87</xdr:row>
+      <xdr:rowOff>251460</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>639461</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>39723</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="15" name="Picture 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A50AEBE2-1D0C-0265-9BB0-4FCCD91EF64A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6896100" y="37155120"/>
+          <a:ext cx="4952381" cy="2257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>449581</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>89181</xdr:colOff>
+      <xdr:row>108</xdr:row>
+      <xdr:rowOff>349696</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="16" name="Picture 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F6D25191-788B-48F9-8094-F5103569B9E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1120141" y="41338500"/>
+          <a:ext cx="5674640" cy="4754056"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>97</xdr:row>
+      <xdr:rowOff>365760</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>643283</xdr:colOff>
+      <xdr:row>107</xdr:row>
+      <xdr:rowOff>270008</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="17" name="Picture 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7F365C54-C53B-468A-93D9-DFFB073F829F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7665720" y="41582340"/>
+          <a:ext cx="4857143" cy="4019048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>109</xdr:row>
+      <xdr:rowOff>274320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>490864</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>216663</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="18" name="Picture 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{34A935DC-7C9C-4259-971D-7C789F59EBAA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="175260" y="46428660"/>
+          <a:ext cx="5009524" cy="4057143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>320040</xdr:colOff>
+      <xdr:row>112</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>178525</xdr:colOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>317922</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Picture 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D7E21CEE-2F32-BEA6-A3A2-AE8DDC5630DD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5013960" y="47647860"/>
+          <a:ext cx="4361905" cy="1704762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>110</xdr:row>
+      <xdr:rowOff>352110</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>465948</xdr:colOff>
+      <xdr:row>119</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{24877EB2-2C9B-7440-A248-082F59164386}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9464040" y="46917930"/>
+          <a:ext cx="4222608" cy="3366450"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>122</xdr:row>
+      <xdr:rowOff>205740</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>149825</xdr:colOff>
+      <xdr:row>128</xdr:row>
+      <xdr:rowOff>155908</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="21" name="Picture 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0E35AD9-34C4-623A-A3AC-8912F7304CE0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId18"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="822960" y="51907440"/>
+          <a:ext cx="5361905" cy="2419048"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>129</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>343627</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A1BC7890-C057-04C2-7331-A0AA8F0624DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId19"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1280160" y="54658260"/>
+          <a:ext cx="2781300" cy="2324827"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>130</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>569029</xdr:colOff>
+      <xdr:row>134</xdr:row>
+      <xdr:rowOff>253145</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="23" name="Picture 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AC98C7A-88DE-A885-75CE-C2C0480E1B3C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId20"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4572000" y="55130700"/>
+          <a:ext cx="4523809" cy="1761905"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1267,10 +1807,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M68"/>
+  <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" workbookViewId="0">
+      <selection activeCell="M122" sqref="M122"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
@@ -1339,45 +1879,45 @@
       </c>
     </row>
     <row r="49" spans="1:13" x14ac:dyDescent="0.8">
-      <c r="A49" s="7" t="s">
+      <c r="A49" s="8" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.8">
-      <c r="A50" s="7"/>
-      <c r="K50" s="8" t="s">
+      <c r="A50" s="8"/>
+      <c r="K50" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="51" spans="1:13" x14ac:dyDescent="0.8">
-      <c r="A51" s="7"/>
+      <c r="A51" s="8"/>
       <c r="L51" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.8">
-      <c r="A52" s="7"/>
+      <c r="A52" s="8"/>
       <c r="L52" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:13" ht="22.8" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A53" s="7"/>
+      <c r="A53" s="8"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.8">
-      <c r="A54" s="7"/>
-      <c r="K54" s="8" t="s">
+      <c r="A54" s="8"/>
+      <c r="K54" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.8">
-      <c r="A55" s="7"/>
+      <c r="A55" s="8"/>
       <c r="L55" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:13" x14ac:dyDescent="0.8">
-      <c r="A56" s="7"/>
+      <c r="A56" s="8"/>
       <c r="L56" s="1" t="s">
         <v>28</v>
       </c>
@@ -1417,19 +1957,34 @@
         <v>36</v>
       </c>
     </row>
-    <row r="65" spans="9:9" x14ac:dyDescent="0.8">
+    <row r="65" spans="2:9" x14ac:dyDescent="0.8">
       <c r="I65" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="67" spans="9:9" x14ac:dyDescent="0.8">
+    <row r="67" spans="2:9" x14ac:dyDescent="0.8">
       <c r="I67" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="68" spans="9:9" x14ac:dyDescent="0.8">
+    <row r="68" spans="2:9" x14ac:dyDescent="0.8">
       <c r="I68" s="1" t="s">
         <v>38</v>
+      </c>
+    </row>
+    <row r="72" spans="2:9" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B72" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="97" spans="2:2" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B97" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="B122" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Form] - Use function for validation
</commit_message>
<xml_diff>
--- a/Tutorial #/Form.xlsx
+++ b/Tutorial #/Form.xlsx
@@ -8,15 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\Flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16F8CE0-B2AD-42EF-B4E2-B92FE3FCE0F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A414C4-44D8-41EB-B494-68CDE3FDDC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Form" sheetId="1" r:id="rId1"/>
-    <sheet name="Single child scroll view proper" sheetId="2" r:id="rId2"/>
+    <sheet name="Form validation" sheetId="1" r:id="rId1"/>
+    <sheet name="Use function for validation" sheetId="3" r:id="rId2"/>
+    <sheet name="Single child scroll view proper" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <r>
       <rPr>
@@ -299,6 +301,23 @@
   <si>
     <t xml:space="preserve">Form එක validate නම් values ටික අරගමු </t>
     <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Set widget as function</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">එකම code නැවත නැවත ලියන්න වෙනවා </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text field කීපයක් use කරනකොට </t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t xml:space="preserve">එක නැතිකරගන්න </t>
+  </si>
+  <si>
+    <t xml:space="preserve">widgets වෙනම functions වලට දාන්න පුළුවන් </t>
   </si>
 </sst>
 </file>
@@ -1452,6 +1471,99 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>358140</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>191877</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>233707</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BBAE133-29F6-C22C-615E-E0D729454380}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="358140" y="801477"/>
+          <a:ext cx="4663440" cy="2777410"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>403860</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>509605</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>121920</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DFA69B8A-D4A1-E12F-8143-2352A95F9C23}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="403860" y="3947160"/>
+          <a:ext cx="5470225" cy="6515100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -1809,8 +1921,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M122"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A115" workbookViewId="0">
-      <selection activeCell="M122" sqref="M122"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
@@ -1999,6 +2111,53 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E1E0AE-D6AE-4C70-AB3F-86D92AFD7D93}">
+  <dimension ref="A1:J7"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.8"/>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="I3" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="J4" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="I6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.8">
+      <c r="J7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EEFCA9-EE7F-4190-8508-BC0C5BFF0AEF}">
   <dimension ref="A1:N15"/>
   <sheetViews>

</xml_diff>

<commit_message>
[Form] - Use Class for validation
</commit_message>
<xml_diff>
--- a/Tutorial #/Form.xlsx
+++ b/Tutorial #/Form.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\development\Flutter_project\Tutorial #\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48A414C4-44D8-41EB-B494-68CDE3FDDC25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61364784-0CF8-4541-8F0F-123BC6757509}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Form validation" sheetId="1" r:id="rId1"/>
     <sheet name="Use function for validation" sheetId="3" r:id="rId2"/>
-    <sheet name="Single child scroll view proper" sheetId="2" r:id="rId3"/>
+    <sheet name="Use Class for validation" sheetId="4" r:id="rId3"/>
+    <sheet name="Single child scroll view proper" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="48">
   <si>
     <r>
       <rPr>
@@ -318,6 +318,10 @@
   </si>
   <si>
     <t xml:space="preserve">widgets වෙනම functions වලට දාන්න පුළුවන් </t>
+  </si>
+  <si>
+    <t>Use Class for validation</t>
+    <phoneticPr fontId="3"/>
   </si>
 </sst>
 </file>
@@ -1564,6 +1568,187 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>248002</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>555174</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>278912</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F17507D8-EC24-9735-258F-69507BD8C6F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="248002" y="769620"/>
+          <a:ext cx="6342212" cy="6557792"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>179432</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>536431</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>48704</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DCBCB1C0-0DA8-7AC5-045A-AD64A008EB1C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7555592" y="914400"/>
+          <a:ext cx="5050919" cy="5359844"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>434340</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>259080</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>390944</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>406601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Picture 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D529127-4811-5DC4-7818-61D82E2FAEC9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="434340" y="7719060"/>
+          <a:ext cx="3309404" cy="5908241"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>532738</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>290731</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>403861</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C2BE450-E606-D611-B190-620E34783B2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4556098" y="7680960"/>
+          <a:ext cx="3110793" cy="5943601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -2114,8 +2299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5E1E0AE-D6AE-4C70-AB3F-86D92AFD7D93}">
   <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
@@ -2158,6 +2343,33 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B14BA7-4A71-43FC-8D69-FD7DE40206B1}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="32.4" x14ac:dyDescent="0.8"/>
+  <cols>
+    <col min="1" max="16384" width="8.796875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="48" x14ac:dyDescent="1.1499999999999999">
+      <c r="A1" s="5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="21" customHeight="1" x14ac:dyDescent="0.8"/>
+  </sheetData>
+  <phoneticPr fontId="3"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10EEFCA9-EE7F-4190-8508-BC0C5BFF0AEF}">
   <dimension ref="A1:N15"/>
   <sheetViews>

</xml_diff>